<commit_message>
Swap location of square and curly brackets
</commit_message>
<xml_diff>
--- a/Key layout.xlsx
+++ b/Key layout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lol_f\Documents\GitHub\Keyboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frleheri\Documents\GitHub\Keyboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F0EB0A-79CB-421B-B4D3-5597CEAC3DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D03E649-77D7-41DF-8FFB-23A22A9E383B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="1730" windowWidth="12680" windowHeight="10190" xr2:uid="{8FB76BC3-2A3C-4BB8-828D-89A98B45AE68}"/>
+    <workbookView xWindow="34929" yWindow="-891" windowWidth="12360" windowHeight="9188" xr2:uid="{8FB76BC3-2A3C-4BB8-828D-89A98B45AE68}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -484,7 +484,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -536,20 +536,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -866,15 +857,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFA44387-4D0A-471D-A3E3-F82BF7F8B165}">
-  <dimension ref="A2:AI30"/>
+  <dimension ref="B2:AI27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:AA30"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.81640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="3.84375" defaultRowHeight="20.05" customHeight="1" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="2" spans="1:35" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="7"/>
       <c r="C2" s="2"/>
       <c r="D2" s="6"/>
@@ -898,14 +889,14 @@
       <c r="V2" s="15"/>
       <c r="W2" s="1"/>
       <c r="X2" s="18"/>
-      <c r="Y2" s="6"/>
+      <c r="Y2" s="1"/>
       <c r="Z2" s="2"/>
       <c r="AA2" s="10"/>
       <c r="AB2" s="11"/>
       <c r="AC2" s="10"/>
       <c r="AD2" s="11"/>
     </row>
-    <row r="3" spans="1:35" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="3"/>
       <c r="C3" s="31"/>
       <c r="D3" s="3"/>
@@ -929,7 +920,7 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="31"/>
     </row>
-    <row r="4" spans="1:35" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="1"/>
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
@@ -973,15 +964,15 @@
       <c r="X4" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="Y4" s="6" t="s">
-        <v>44</v>
+      <c r="Y4" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="Z4" s="20" t="s">
         <v>92</v>
       </c>
       <c r="AC4" s="27"/>
     </row>
-    <row r="5" spans="1:35" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="5" t="s">
         <v>62</v>
       </c>
@@ -1050,13 +1041,13 @@
         <v>84</v>
       </c>
       <c r="Y5" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="Z5" s="25" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:35" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="14"/>
       <c r="C6" s="4"/>
       <c r="D6" s="1"/>
@@ -1111,7 +1102,7 @@
       <c r="AH6" s="11"/>
       <c r="AI6" s="11"/>
     </row>
-    <row r="7" spans="1:35" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="3" t="s">
         <v>38</v>
       </c>
@@ -1186,7 +1177,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:35" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="18" t="s">
         <v>78</v>
@@ -1236,15 +1227,15 @@
       <c r="X8" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="Y8" s="1" t="s">
-        <v>46</v>
+      <c r="Y8" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="Z8" s="18" t="s">
         <v>97</v>
       </c>
       <c r="AC8" s="22"/>
     </row>
-    <row r="9" spans="1:35" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="3" t="s">
         <v>96</v>
       </c>
@@ -1287,13 +1278,13 @@
       </c>
       <c r="X9" s="26"/>
       <c r="Y9" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Z9" s="26" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:35" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="4"/>
       <c r="D10" s="1"/>
@@ -1328,7 +1319,7 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="2"/>
     </row>
-    <row r="11" spans="1:35" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="3"/>
       <c r="D11" s="16"/>
       <c r="F11" s="3"/>
@@ -1355,7 +1346,7 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="19"/>
     </row>
-    <row r="12" spans="1:35" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -1380,469 +1371,77 @@
       <c r="X12" s="4"/>
       <c r="Z12" s="4"/>
     </row>
-    <row r="15" spans="1:35" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="33"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
-      <c r="K15" s="33"/>
-      <c r="L15" s="33"/>
-      <c r="M15" s="33"/>
-      <c r="N15" s="33"/>
-      <c r="O15" s="33"/>
-      <c r="P15" s="33"/>
-      <c r="Q15" s="33"/>
-      <c r="R15" s="33"/>
-      <c r="S15" s="33"/>
-      <c r="T15" s="33"/>
-      <c r="U15" s="33"/>
-      <c r="V15" s="33"/>
-      <c r="W15" s="33"/>
-      <c r="X15" s="33"/>
-      <c r="Y15" s="33"/>
-      <c r="Z15" s="33"/>
-      <c r="AA15" s="33"/>
-    </row>
-    <row r="16" spans="1:35" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="33"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
-      <c r="K16" s="33"/>
-      <c r="L16" s="33"/>
-      <c r="M16" s="33"/>
-      <c r="N16" s="36"/>
-      <c r="O16" s="33"/>
-      <c r="P16" s="33"/>
-      <c r="Q16" s="33"/>
-      <c r="R16" s="33"/>
-      <c r="S16" s="33"/>
-      <c r="T16" s="37"/>
-      <c r="U16" s="33"/>
-      <c r="V16" s="37"/>
-      <c r="W16" s="38"/>
-      <c r="X16" s="37"/>
-      <c r="Y16" s="38"/>
-      <c r="Z16" s="33"/>
-      <c r="AA16" s="38"/>
-    </row>
-    <row r="17" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
-      <c r="K17" s="33"/>
-      <c r="L17" s="33"/>
-      <c r="M17" s="33"/>
-      <c r="N17" s="33"/>
-      <c r="O17" s="33"/>
-      <c r="P17" s="33"/>
-      <c r="Q17" s="33"/>
-      <c r="R17" s="33"/>
-      <c r="S17" s="33"/>
-      <c r="T17" s="33"/>
-      <c r="U17" s="33"/>
-      <c r="V17" s="33"/>
-      <c r="W17" s="33"/>
-      <c r="X17" s="33"/>
-      <c r="Y17" s="33"/>
-      <c r="Z17" s="33"/>
-      <c r="AA17" s="33"/>
-    </row>
-    <row r="18" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="37"/>
-      <c r="L18" s="33"/>
-      <c r="M18" s="33"/>
-      <c r="N18" s="33"/>
-      <c r="O18" s="33"/>
-      <c r="P18" s="33"/>
-      <c r="Q18" s="33"/>
-      <c r="R18" s="37"/>
-      <c r="S18" s="33"/>
-      <c r="T18" s="37"/>
-      <c r="U18" s="33"/>
-      <c r="V18" s="37"/>
-      <c r="W18" s="33"/>
-      <c r="X18" s="37"/>
-      <c r="Y18" s="33"/>
-      <c r="Z18" s="33"/>
-      <c r="AA18" s="33"/>
-    </row>
-    <row r="19" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="33"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33"/>
-      <c r="N19" s="33"/>
-      <c r="O19" s="33"/>
-      <c r="P19" s="33"/>
-      <c r="Q19" s="33"/>
-      <c r="R19" s="39"/>
-      <c r="S19" s="33"/>
-      <c r="T19" s="33"/>
-      <c r="U19" s="33"/>
-      <c r="V19" s="39"/>
-      <c r="W19" s="33"/>
-      <c r="X19" s="33"/>
-      <c r="Y19" s="33"/>
-      <c r="Z19" s="39"/>
-      <c r="AA19" s="33"/>
-    </row>
-    <row r="20" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="33"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="33"/>
-      <c r="L20" s="33"/>
-      <c r="M20" s="33"/>
-      <c r="N20" s="33"/>
-      <c r="O20" s="33"/>
-      <c r="P20" s="33"/>
-      <c r="Q20" s="33"/>
-      <c r="R20" s="37"/>
-      <c r="S20" s="33"/>
-      <c r="T20" s="37"/>
-      <c r="U20" s="33"/>
-      <c r="V20" s="37"/>
-      <c r="W20" s="33"/>
-      <c r="X20" s="37"/>
-      <c r="Y20" s="33"/>
-      <c r="Z20" s="33"/>
-      <c r="AA20" s="33"/>
-    </row>
-    <row r="21" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="33"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
-      <c r="N21" s="33"/>
-      <c r="O21" s="33"/>
-      <c r="P21" s="33"/>
-      <c r="Q21" s="33"/>
-      <c r="R21" s="39"/>
-      <c r="S21" s="33"/>
-      <c r="T21" s="39"/>
-      <c r="U21" s="33"/>
-      <c r="V21" s="39"/>
-      <c r="W21" s="33"/>
-      <c r="X21" s="39"/>
-      <c r="Y21" s="33"/>
-      <c r="Z21" s="39"/>
-      <c r="AA21" s="33"/>
-    </row>
-    <row r="22" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="33"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
-      <c r="O22" s="33"/>
-      <c r="P22" s="33"/>
-      <c r="Q22" s="33"/>
-      <c r="R22" s="37"/>
-      <c r="S22" s="33"/>
-      <c r="T22" s="37"/>
-      <c r="U22" s="33"/>
-      <c r="V22" s="37"/>
-      <c r="W22" s="33"/>
-      <c r="X22" s="37"/>
-      <c r="Y22" s="33"/>
-      <c r="Z22" s="33"/>
-      <c r="AA22" s="33"/>
-    </row>
-    <row r="23" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="33"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="33"/>
-      <c r="M23" s="33"/>
-      <c r="N23" s="33"/>
-      <c r="O23" s="33"/>
-      <c r="P23" s="33"/>
-      <c r="Q23" s="33"/>
-      <c r="R23" s="33"/>
-      <c r="S23" s="33"/>
-      <c r="T23" s="33"/>
-      <c r="U23" s="33"/>
-      <c r="V23" s="33"/>
-      <c r="W23" s="33"/>
-      <c r="X23" s="33"/>
-      <c r="Y23" s="33"/>
-      <c r="Z23" s="39"/>
-      <c r="AA23" s="33"/>
-    </row>
-    <row r="24" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="33"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="33"/>
-      <c r="N24" s="33"/>
-      <c r="O24" s="33"/>
-      <c r="P24" s="33"/>
-      <c r="Q24" s="33"/>
-      <c r="R24" s="33"/>
-      <c r="S24" s="37"/>
-      <c r="T24" s="33"/>
-      <c r="U24" s="33"/>
-      <c r="V24" s="37"/>
-      <c r="W24" s="33"/>
-      <c r="X24" s="37"/>
-      <c r="Y24" s="33"/>
-      <c r="Z24" s="37"/>
-      <c r="AA24" s="33"/>
-    </row>
-    <row r="25" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="33"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="37"/>
-      <c r="K25" s="33"/>
-      <c r="L25" s="33"/>
-      <c r="M25" s="33"/>
-      <c r="N25" s="33"/>
-      <c r="O25" s="33"/>
-      <c r="P25" s="33"/>
-      <c r="Q25" s="33"/>
-      <c r="R25" s="33"/>
-      <c r="S25" s="33"/>
-      <c r="T25" s="33"/>
-      <c r="U25" s="33"/>
-      <c r="V25" s="33"/>
-      <c r="W25" s="33"/>
-      <c r="X25" s="33"/>
-      <c r="Y25" s="33"/>
-      <c r="Z25" s="33"/>
-      <c r="AA25" s="33"/>
-    </row>
-    <row r="26" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="33"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="33"/>
-      <c r="K26" s="33"/>
-      <c r="L26" s="33"/>
-      <c r="M26" s="33"/>
-      <c r="N26" s="33"/>
-      <c r="O26" s="33"/>
-      <c r="P26" s="33"/>
-      <c r="Q26" s="33"/>
-      <c r="R26" s="33"/>
-      <c r="S26" s="33"/>
-      <c r="T26" s="33"/>
-      <c r="U26" s="33"/>
-      <c r="V26" s="33"/>
-      <c r="W26" s="33"/>
-      <c r="X26" s="33"/>
-      <c r="Y26" s="33"/>
-      <c r="Z26" s="33"/>
-      <c r="AA26" s="33"/>
-    </row>
-    <row r="27" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="33"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="37"/>
-      <c r="K27" s="33"/>
-      <c r="L27" s="33"/>
-      <c r="M27" s="33"/>
-      <c r="N27" s="33"/>
-      <c r="O27" s="33"/>
-      <c r="P27" s="33"/>
-      <c r="Q27" s="39"/>
-      <c r="R27" s="33"/>
-      <c r="S27" s="33"/>
-      <c r="T27" s="33"/>
-      <c r="U27" s="33"/>
-      <c r="V27" s="33"/>
-      <c r="W27" s="33"/>
-      <c r="X27" s="33"/>
-      <c r="Y27" s="33"/>
-      <c r="Z27" s="33"/>
-      <c r="AA27" s="33"/>
-    </row>
-    <row r="28" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="33"/>
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33"/>
-      <c r="J28" s="33"/>
-      <c r="K28" s="33"/>
-      <c r="L28" s="33"/>
-      <c r="M28" s="33"/>
-      <c r="N28" s="33"/>
-      <c r="O28" s="33"/>
-      <c r="P28" s="33"/>
-      <c r="Q28" s="33"/>
-      <c r="R28" s="33"/>
-      <c r="S28" s="33"/>
-      <c r="T28" s="33"/>
-      <c r="U28" s="33"/>
-      <c r="V28" s="33"/>
-      <c r="W28" s="33"/>
-      <c r="X28" s="33"/>
-      <c r="Y28" s="33"/>
-      <c r="Z28" s="33"/>
-      <c r="AA28" s="33"/>
-    </row>
-    <row r="29" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="33"/>
-      <c r="B29" s="33"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
-      <c r="J29" s="33"/>
-      <c r="K29" s="33"/>
-      <c r="L29" s="33"/>
-      <c r="M29" s="33"/>
-      <c r="N29" s="33"/>
-      <c r="O29" s="33"/>
-      <c r="P29" s="33"/>
-      <c r="Q29" s="33"/>
-      <c r="R29" s="33"/>
-      <c r="S29" s="33"/>
-      <c r="T29" s="33"/>
-      <c r="U29" s="33"/>
-      <c r="V29" s="33"/>
-      <c r="W29" s="33"/>
-      <c r="X29" s="33"/>
-      <c r="Y29" s="33"/>
-      <c r="Z29" s="33"/>
-      <c r="AA29" s="33"/>
-    </row>
-    <row r="30" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="33"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
-      <c r="K30" s="33"/>
-      <c r="L30" s="33"/>
-      <c r="M30" s="33"/>
-      <c r="N30" s="33"/>
-      <c r="O30" s="33"/>
-      <c r="P30" s="33"/>
-      <c r="Q30" s="33"/>
-      <c r="R30" s="33"/>
-      <c r="S30" s="33"/>
-      <c r="T30" s="33"/>
-      <c r="U30" s="33"/>
-      <c r="V30" s="33"/>
-      <c r="W30" s="33"/>
-      <c r="X30" s="33"/>
-      <c r="Y30" s="33"/>
-      <c r="Z30" s="33"/>
-      <c r="AA30" s="33"/>
+    <row r="15" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="33"/>
+    </row>
+    <row r="16" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="34"/>
+      <c r="C16" s="11"/>
+      <c r="G16" s="22"/>
+      <c r="N16" s="11"/>
+      <c r="T16" s="22"/>
+      <c r="V16" s="22"/>
+      <c r="W16" s="10"/>
+      <c r="X16" s="22"/>
+      <c r="Y16" s="10"/>
+      <c r="AA16" s="10"/>
+    </row>
+    <row r="18" spans="3:26" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="R18" s="22"/>
+      <c r="T18" s="22"/>
+      <c r="V18" s="22"/>
+      <c r="X18" s="22"/>
+    </row>
+    <row r="19" spans="3:26" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="R19" s="23"/>
+      <c r="V19" s="23"/>
+      <c r="Z19" s="23"/>
+    </row>
+    <row r="20" spans="3:26" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="R20" s="22"/>
+      <c r="T20" s="22"/>
+      <c r="V20" s="22"/>
+      <c r="X20" s="22"/>
+    </row>
+    <row r="21" spans="3:26" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="R21" s="23"/>
+      <c r="T21" s="23"/>
+      <c r="V21" s="23"/>
+      <c r="X21" s="23"/>
+      <c r="Z21" s="23"/>
+    </row>
+    <row r="22" spans="3:26" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="G22" s="22"/>
+      <c r="R22" s="22"/>
+      <c r="T22" s="22"/>
+      <c r="V22" s="22"/>
+      <c r="X22" s="22"/>
+    </row>
+    <row r="23" spans="3:26" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Z23" s="23"/>
+    </row>
+    <row r="24" spans="3:26" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="S24" s="22"/>
+      <c r="V24" s="22"/>
+      <c r="X24" s="22"/>
+      <c r="Z24" s="22"/>
+    </row>
+    <row r="25" spans="3:26" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D25" s="35"/>
+      <c r="F25" s="35"/>
+      <c r="J25" s="22"/>
+    </row>
+    <row r="27" spans="3:26" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="J27" s="22"/>
+      <c r="Q27" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Remove usage of the three side keys
</commit_message>
<xml_diff>
--- a/Key layout.xlsx
+++ b/Key layout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frleheri\Documents\GitHub\Keyboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D03E649-77D7-41DF-8FFB-23A22A9E383B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CD93CF-B0F3-4443-A439-5BE78F14D974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34929" yWindow="-891" windowWidth="12360" windowHeight="9188" xr2:uid="{8FB76BC3-2A3C-4BB8-828D-89A98B45AE68}"/>
+    <workbookView xWindow="35443" yWindow="-2297" windowWidth="13174" windowHeight="10148" xr2:uid="{8FB76BC3-2A3C-4BB8-828D-89A98B45AE68}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="99">
   <si>
     <t>A</t>
   </si>
@@ -328,14 +328,17 @@
     <t xml:space="preserve">⊞ </t>
   </si>
   <si>
-    <t>&lt;&gt;</t>
+    <t>&lt;</t>
+  </si>
+  <si>
+    <t>&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -368,6 +371,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -484,7 +494,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -523,7 +533,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
@@ -543,6 +552,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -860,7 +875,7 @@
   <dimension ref="B2:AI27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.84375" defaultRowHeight="20.05" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -879,10 +894,10 @@
       <c r="L2" s="6"/>
       <c r="M2" s="2"/>
       <c r="N2" s="11"/>
-      <c r="O2" s="32"/>
+      <c r="O2" s="31"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="4"/>
-      <c r="R2" s="30"/>
+      <c r="R2" s="29"/>
       <c r="S2" s="1"/>
       <c r="T2" s="20"/>
       <c r="U2" s="4"/>
@@ -898,116 +913,120 @@
     </row>
     <row r="3" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="3"/>
-      <c r="C3" s="31"/>
+      <c r="C3" s="30"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="31"/>
+      <c r="E3" s="30"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="31"/>
+      <c r="G3" s="30"/>
       <c r="H3" s="3"/>
-      <c r="I3" s="31"/>
+      <c r="I3" s="30"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="31"/>
+      <c r="K3" s="30"/>
       <c r="L3" s="3"/>
-      <c r="M3" s="31"/>
+      <c r="M3" s="30"/>
       <c r="O3" s="3"/>
-      <c r="P3" s="31"/>
+      <c r="P3" s="30"/>
       <c r="R3" s="11"/>
       <c r="S3" s="3"/>
-      <c r="T3" s="31"/>
+      <c r="T3" s="30"/>
       <c r="V3" s="11"/>
       <c r="W3" s="3"/>
-      <c r="X3" s="31"/>
+      <c r="X3" s="30"/>
       <c r="Y3" s="3"/>
-      <c r="Z3" s="31"/>
+      <c r="Z3" s="30"/>
     </row>
     <row r="4" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="1"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="1"/>
+      <c r="D4" s="35"/>
       <c r="E4" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="F4" s="35"/>
       <c r="G4" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="H4" s="1"/>
+      <c r="H4" s="35"/>
       <c r="I4" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="J4" s="1"/>
+      <c r="J4" s="35"/>
       <c r="K4" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="L4" s="1"/>
+        <v>78</v>
+      </c>
+      <c r="L4" s="35" t="s">
+        <v>91</v>
+      </c>
       <c r="M4" s="21" t="s">
         <v>77</v>
       </c>
       <c r="N4" s="8"/>
-      <c r="O4" s="4"/>
+      <c r="O4" s="36" t="s">
+        <v>89</v>
+      </c>
       <c r="P4" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="Q4" s="1"/>
+      <c r="Q4" s="35" t="s">
+        <v>44</v>
+      </c>
       <c r="R4" s="15">
         <v>7</v>
       </c>
-      <c r="S4" s="1"/>
+      <c r="S4" s="35" t="s">
+        <v>48</v>
+      </c>
       <c r="T4" s="15">
         <v>8</v>
       </c>
-      <c r="U4" s="24"/>
+      <c r="U4" s="35" t="s">
+        <v>46</v>
+      </c>
       <c r="V4" s="18">
         <v>9</v>
       </c>
-      <c r="W4" s="24"/>
+      <c r="W4" s="35" t="s">
+        <v>98</v>
+      </c>
       <c r="X4" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="Y4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z4" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="AC4" s="27"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="20"/>
+      <c r="AC4" s="26"/>
     </row>
     <row r="5" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="31" t="s">
-        <v>26</v>
-      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="31" t="s">
-        <v>27</v>
+      <c r="E5" s="30" t="s">
+        <v>26</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="31" t="s">
-        <v>28</v>
+      <c r="G5" s="30" t="s">
+        <v>27</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="31" t="s">
-        <v>29</v>
+      <c r="I5" s="30" t="s">
+        <v>28</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="31" t="s">
-        <v>30</v>
+      <c r="K5" s="30" t="s">
+        <v>29</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="31" t="s">
-        <v>31</v>
+      <c r="M5" s="30" t="s">
+        <v>62</v>
       </c>
       <c r="N5" s="8"/>
       <c r="O5" t="s">
@@ -1040,104 +1059,104 @@
       <c r="X5" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="Y5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z5" s="25" t="s">
-        <v>82</v>
-      </c>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="24"/>
     </row>
     <row r="6" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="14"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="1"/>
+      <c r="D6" s="35"/>
       <c r="E6" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="35"/>
       <c r="G6" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="H6" s="1"/>
+      <c r="H6" s="35"/>
       <c r="I6" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="J6" s="1"/>
+      <c r="J6" s="35"/>
       <c r="K6" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="L6" s="1"/>
+      <c r="L6" s="35" t="s">
+        <v>92</v>
+      </c>
       <c r="M6" s="15" t="s">
         <v>76</v>
       </c>
       <c r="N6" s="8"/>
-      <c r="O6" s="4"/>
+      <c r="O6" s="36" t="s">
+        <v>81</v>
+      </c>
       <c r="P6" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="Q6" s="1"/>
+      <c r="Q6" s="35" t="s">
+        <v>43</v>
+      </c>
       <c r="R6" s="15">
         <v>4</v>
       </c>
-      <c r="S6" s="1"/>
+      <c r="S6" s="35" t="s">
+        <v>47</v>
+      </c>
       <c r="T6" s="15">
         <v>5</v>
       </c>
-      <c r="U6" s="24"/>
+      <c r="U6" s="35" t="s">
+        <v>45</v>
+      </c>
       <c r="V6" s="18">
         <v>6</v>
       </c>
-      <c r="W6" s="24"/>
+      <c r="W6" s="35" t="s">
+        <v>97</v>
+      </c>
       <c r="X6" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="Y6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z6" s="18" t="s">
-        <v>90</v>
-      </c>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="18"/>
       <c r="AC6" s="22"/>
       <c r="AG6" s="10"/>
       <c r="AH6" s="11"/>
       <c r="AI6" s="11"/>
     </row>
     <row r="7" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="31" t="s">
-        <v>32</v>
-      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>33</v>
+      <c r="E7" s="30" t="s">
+        <v>30</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="31" t="s">
-        <v>34</v>
+      <c r="G7" s="30" t="s">
+        <v>31</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="11" t="s">
-        <v>35</v>
+      <c r="I7" s="30" t="s">
+        <v>32</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="31" t="s">
-        <v>36</v>
+      <c r="K7" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="M7" s="31" t="s">
-        <v>37</v>
+      <c r="M7" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="N7" s="8"/>
       <c r="O7" t="s">
@@ -1170,42 +1189,34 @@
       <c r="X7" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="Y7" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z7" s="25" t="s">
-        <v>83</v>
-      </c>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="24"/>
     </row>
     <row r="8" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="H8" s="1"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="35"/>
       <c r="I8" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="J8" s="1"/>
+      <c r="J8" s="35"/>
       <c r="K8" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="L8" s="1"/>
+      <c r="L8" s="35" t="s">
+        <v>90</v>
+      </c>
       <c r="M8" s="15" t="s">
         <v>79</v>
       </c>
       <c r="N8" s="8"/>
-      <c r="O8" s="4"/>
+      <c r="O8" s="36"/>
       <c r="P8" s="15"/>
-      <c r="Q8" s="1"/>
+      <c r="Q8" s="35"/>
       <c r="R8" s="15">
         <v>1</v>
       </c>
@@ -1227,35 +1238,41 @@
       <c r="X8" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="Y8" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z8" s="18" t="s">
-        <v>97</v>
-      </c>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="18"/>
       <c r="AC8" s="22"/>
     </row>
     <row r="9" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="3" t="s">
-        <v>96</v>
-      </c>
+      <c r="B9" s="3"/>
       <c r="D9" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="E9" s="30" t="s">
+        <v>34</v>
+      </c>
       <c r="F9" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="G9" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="H9" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="I9" s="30" t="s">
+        <v>36</v>
+      </c>
       <c r="J9" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="K9" s="30" t="s">
+        <v>37</v>
+      </c>
       <c r="L9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M9" s="23" t="s">
-        <v>57</v>
+      <c r="M9" s="11" t="s">
+        <v>96</v>
       </c>
       <c r="N9" s="8"/>
       <c r="O9" s="3" t="s">
@@ -1267,22 +1284,29 @@
       <c r="Q9" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="R9" s="23" t="s">
+        <v>57</v>
+      </c>
       <c r="S9" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="T9" s="24" t="s">
+        <v>82</v>
+      </c>
       <c r="U9" s="3" t="s">
         <v>49</v>
       </c>
+      <c r="V9" s="24" t="s">
+        <v>83</v>
+      </c>
       <c r="W9" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="X9" s="26"/>
-      <c r="Y9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z9" s="26" t="s">
+      <c r="X9" s="25" t="s">
         <v>86</v>
       </c>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="25"/>
     </row>
     <row r="10" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
@@ -1301,7 +1325,7 @@
       </c>
       <c r="N10" s="8"/>
       <c r="O10" s="4"/>
-      <c r="P10" s="29" t="s">
+      <c r="P10" s="28" t="s">
         <v>60</v>
       </c>
       <c r="Q10" s="1"/>
@@ -1315,7 +1339,7 @@
       <c r="U10" s="1"/>
       <c r="V10" s="18"/>
       <c r="W10" s="1"/>
-      <c r="X10" s="28"/>
+      <c r="X10" s="27"/>
       <c r="Y10" s="1"/>
       <c r="Z10" s="2"/>
     </row>
@@ -1371,11 +1395,23 @@
       <c r="X12" s="4"/>
       <c r="Z12" s="4"/>
     </row>
+    <row r="13" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="38"/>
+    </row>
+    <row r="14" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+    </row>
     <row r="15" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="33"/>
+      <c r="B15" s="32"/>
     </row>
     <row r="16" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="34"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="11"/>
       <c r="G16" s="22"/>
       <c r="N16" s="11"/>
@@ -1435,8 +1471,8 @@
       <c r="Z24" s="22"/>
     </row>
     <row r="25" spans="3:26" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="D25" s="35"/>
-      <c r="F25" s="35"/>
+      <c r="D25" s="34"/>
+      <c r="F25" s="34"/>
       <c r="J25" s="22"/>
     </row>
     <row r="27" spans="3:26" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Add key to hold space and move "_"
</commit_message>
<xml_diff>
--- a/Key layout.xlsx
+++ b/Key layout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frleheri\Documents\GitHub\Keyboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Github\Keyboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5F2A17-1D79-48EC-B895-95E925183E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077B3B91-EF39-41C5-8747-4842B3905FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1714" yWindow="1414" windowWidth="24369" windowHeight="15146" xr2:uid="{8FB76BC3-2A3C-4BB8-828D-89A98B45AE68}"/>
+    <workbookView xWindow="5980" yWindow="1720" windowWidth="30890" windowHeight="18330" xr2:uid="{8FB76BC3-2A3C-4BB8-828D-89A98B45AE68}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="98">
   <si>
     <t>A</t>
   </si>
@@ -326,6 +326,9 @@
   </si>
   <si>
     <t>&gt;</t>
+  </si>
+  <si>
+    <t>Space</t>
   </si>
 </sst>
 </file>
@@ -521,9 +524,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -561,7 +564,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -667,7 +670,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -809,7 +812,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -820,12 +823,12 @@
   <dimension ref="B2:AI27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AK7" sqref="AK7"/>
+      <selection activeCell="AA18" sqref="AA18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.84375" defaultRowHeight="20.05" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="3.81640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:35" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="17"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6"/>
@@ -845,7 +848,7 @@
       <c r="AC2" s="5"/>
       <c r="AD2" s="6"/>
     </row>
-    <row r="3" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:35" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C3" s="6"/>
       <c r="E3" s="6"/>
       <c r="G3" s="6"/>
@@ -866,7 +869,7 @@
       <c r="AA3" s="6"/>
       <c r="AC3" s="6"/>
     </row>
-    <row r="4" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:35" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F4" s="19"/>
       <c r="G4" s="9" t="s">
         <v>55</v>
@@ -912,7 +915,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:35" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C5" s="6"/>
       <c r="D5" s="19"/>
       <c r="E5" s="9" t="s">
@@ -971,7 +974,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:35" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="12"/>
       <c r="D6" s="3" t="s">
         <v>0</v>
@@ -1033,7 +1036,7 @@
       <c r="AH6" s="6"/>
       <c r="AI6" s="6"/>
     </row>
-    <row r="7" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:35" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C7" s="6"/>
       <c r="D7" s="19"/>
       <c r="E7" s="9" t="s">
@@ -1092,7 +1095,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:35" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C8" s="12"/>
       <c r="D8" s="3" t="s">
         <v>10</v>
@@ -1101,7 +1104,9 @@
         <v>30</v>
       </c>
       <c r="F8" s="19"/>
-      <c r="G8" s="9"/>
+      <c r="G8" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="H8" s="4" t="s">
         <v>22</v>
       </c>
@@ -1116,7 +1121,7 @@
         <v>88</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="T8" s="19"/>
       <c r="U8" s="9"/>
@@ -1141,7 +1146,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:35" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D9" s="19"/>
       <c r="E9" s="9"/>
       <c r="F9" s="4" t="s">
@@ -1183,7 +1188,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:35" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D10" s="3" t="s">
         <v>20</v>
       </c>
@@ -1218,7 +1223,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:35" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D11" s="18"/>
       <c r="J11" s="3" t="s">
         <v>42</v>
@@ -1243,15 +1248,15 @@
       </c>
       <c r="W11" s="10"/>
     </row>
-    <row r="13" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:35" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
     </row>
-    <row r="15" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:35" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="16"/>
     </row>
-    <row r="16" spans="2:35" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:35" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="17"/>
       <c r="C16" s="6"/>
       <c r="G16" s="12"/>
@@ -1263,7 +1268,7 @@
       <c r="Y16" s="5"/>
       <c r="AA16" s="5"/>
     </row>
-    <row r="18" spans="3:26" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="3:26" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C18" s="12"/>
       <c r="G18" s="12"/>
       <c r="I18" s="12"/>
@@ -1273,12 +1278,12 @@
       <c r="V18" s="12"/>
       <c r="X18" s="12"/>
     </row>
-    <row r="19" spans="3:26" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="3:26" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="R19" s="13"/>
       <c r="V19" s="13"/>
       <c r="Z19" s="13"/>
     </row>
-    <row r="20" spans="3:26" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="3:26" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C20" s="12"/>
       <c r="E20" s="12"/>
       <c r="G20" s="12"/>
@@ -1288,35 +1293,35 @@
       <c r="V20" s="12"/>
       <c r="X20" s="12"/>
     </row>
-    <row r="21" spans="3:26" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="3:26" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="R21" s="13"/>
       <c r="T21" s="13"/>
       <c r="V21" s="13"/>
       <c r="X21" s="13"/>
       <c r="Z21" s="13"/>
     </row>
-    <row r="22" spans="3:26" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="3:26" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G22" s="12"/>
       <c r="R22" s="12"/>
       <c r="T22" s="12"/>
       <c r="V22" s="12"/>
       <c r="X22" s="12"/>
     </row>
-    <row r="23" spans="3:26" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="3:26" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="Z23" s="13"/>
     </row>
-    <row r="24" spans="3:26" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="3:26" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="S24" s="12"/>
       <c r="V24" s="12"/>
       <c r="X24" s="12"/>
       <c r="Z24" s="12"/>
     </row>
-    <row r="25" spans="3:26" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="3:26" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D25" s="18"/>
       <c r="F25" s="18"/>
       <c r="J25" s="12"/>
     </row>
-    <row r="27" spans="3:26" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="3:26" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J27" s="12"/>
       <c r="Q27" s="13"/>
     </row>

</xml_diff>